<commit_message>
add some new words
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="610">
   <si>
     <t>expose</t>
   </si>
@@ -1438,13 +1438,421 @@
   </si>
   <si>
     <t xml:space="preserve">vt.发射; [计算机]开始（应用程序）; 发动; 开展（活动、计划等）; vi.投入; 着手进行; 热衷于…; </t>
+  </si>
+  <si>
+    <t>confluence </t>
+  </si>
+  <si>
+    <t>[ˈkɑnfluəns]</t>
+  </si>
+  <si>
+    <t>n.&lt;术&gt;（河流的）汇合处; 汇流处; &lt;正&gt;（事物的）汇合; 汇流;</t>
+  </si>
+  <si>
+    <t>interest</t>
+  </si>
+  <si>
+    <t>[ˈɪntrɪst, -tərɪst, -ˌtrɛst]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n.兴趣，爱好; 利害关系，利益; 利息; 趣味，感兴趣的事; vt.使产生兴趣; 使参与，使加入; 引起…的意愿; 使产生关系; </t>
+  </si>
+  <si>
+    <t>overdo</t>
+  </si>
+  <si>
+    <t>[ˌoʊvərˈdu:]</t>
+  </si>
+  <si>
+    <t>vt.做得过分; 使过于疲劳; 夸张; 耗尽; </t>
+  </si>
+  <si>
+    <t>shore</t>
+  </si>
+  <si>
+    <t>[ʃɔr, ʃor]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n.岸; 滨; 国家（尤指濒海国家）; 支柱; vt.支撑; 支持; </t>
+  </si>
+  <si>
+    <t>offshore</t>
+  </si>
+  <si>
+    <t>[ˌɔ:fˈʃɔ:(r)]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adj.离开海岸的; 近海的; 海外的，国外的; adv.（指风）向海的，离岸的; </t>
+  </si>
+  <si>
+    <t>in advance</t>
+  </si>
+  <si>
+    <t>在前头; 预先，事先; 提前; 先期; </t>
+  </si>
+  <si>
+    <t>approximate</t>
+  </si>
+  <si>
+    <t>[əˈprɑksəmɪt]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adj.约莫的，大概的; 极相似的; [植]相近但不连接的; vi.接近于; 近似于; vt.靠近; 使接近; 使结合; </t>
+  </si>
+  <si>
+    <t>minimize</t>
+  </si>
+  <si>
+    <t>vt.把…减至最低数量[程度]; 对（某事物）作最低估计，极力贬低（某事物）的价值[重要性]; 极度轻视; </t>
+  </si>
+  <si>
+    <t>[ˈmɪnəˌmaɪz]</t>
+  </si>
+  <si>
+    <t>fantasy</t>
+  </si>
+  <si>
+    <t>[ˈfæntəsi, -zi]</t>
+  </si>
+  <si>
+    <t>n.幻想; 空想的产物; 幻想作品; 非正式的货币; </t>
+  </si>
+  <si>
+    <t>nutrition</t>
+  </si>
+  <si>
+    <t>[nuˈtrɪʃən, nju-]</t>
+  </si>
+  <si>
+    <t>n.营养，滋养; 营养品; 营养学; 食物; </t>
+  </si>
+  <si>
+    <t>powder</t>
+  </si>
+  <si>
+    <t>[ˈpaʊdɚ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n.粉，粉末; 粉状物质; vt.在…搽粉; </t>
+  </si>
+  <si>
+    <t>protein</t>
+  </si>
+  <si>
+    <t>[ˈprəʊˌtiːn]</t>
+  </si>
+  <si>
+    <t>n.[化]朊，蛋白（质）; </t>
+  </si>
+  <si>
+    <t>nutrilite</t>
+  </si>
+  <si>
+    <t>['nju:trɪlaɪt]</t>
+  </si>
+  <si>
+    <t>n.营养物; </t>
+  </si>
+  <si>
+    <t>artistry</t>
+  </si>
+  <si>
+    <t>['ɑ:rtɪstrɪ]</t>
+  </si>
+  <si>
+    <t>n.艺术之性质; 技艺; </t>
+  </si>
+  <si>
+    <t>premium</t>
+  </si>
+  <si>
+    <t>[ˈprimiəm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n.额外费用; 保险费; 附加费; adj.高昂的; 优质的; </t>
+  </si>
+  <si>
+    <t>retail</t>
+  </si>
+  <si>
+    <t>[ˈriˌtel]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n.零售; vt.零售; 零卖; 转述; 传播; </t>
+  </si>
+  <si>
+    <t>fundamental </t>
+  </si>
+  <si>
+    <t>[ˌfʌndəˈmɛntl]</t>
+  </si>
+  <si>
+    <t>adj.基础的，基本的，根本的，重要的，原始的，主要的，十分重大的</t>
+  </si>
+  <si>
+    <t xml:space="preserve">correlate </t>
+  </si>
+  <si>
+    <t>[ˈkɔrəˌlet, ˈkɑr-]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v.使互相关联; 联系; n.相关物; 相关联的人; adj.相关的; 相应特点的; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">minimum </t>
+  </si>
+  <si>
+    <t>[ˈmɪnəməm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n.最低限度; 最小量; 最低消费; [数]极小值; adj.最低的; 最小的; 最少的; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">separate </t>
+  </si>
+  <si>
+    <t>['sepəreɪt]</t>
+  </si>
+  <si>
+    <t>adj.单独的; 分开的，分离的; 不同的; 不相关的; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">capitalize </t>
+  </si>
+  <si>
+    <t>[ˈkæpɪtl:ˌaɪz]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vt.用大写字母写或印刷; 使…资本化; 估计…的价值; 把…定为首都; vi.利用; 积累资本; </t>
+  </si>
+  <si>
+    <t>preposition</t>
+  </si>
+  <si>
+    <t>[ˌprɛpəˈzɪʃən]</t>
+  </si>
+  <si>
+    <t>n.介词; 前置词; </t>
+  </si>
+  <si>
+    <t>motto</t>
+  </si>
+  <si>
+    <t>[ˈmɑto]</t>
+  </si>
+  <si>
+    <t>n.座右铭; 格言; 箴言; 主题句; </t>
+  </si>
+  <si>
+    <t>composite </t>
+  </si>
+  <si>
+    <t>[kəmˈpɑzɪt]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adj.混合成的，综合成的; [建]综合式的; [数]可分解的; [植]菊科的; n.合成物，混合物，复合材料; [植]菊科植物; </t>
+  </si>
+  <si>
+    <t>purchase</t>
+  </si>
+  <si>
+    <t>['pɜ:tʃəs]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v.购买; 采购; 换得; 依靠机械力移动; n.购买; 购买行为; 购置物; 紧握; </t>
+  </si>
+  <si>
+    <t>inner mongolia</t>
+  </si>
+  <si>
+    <t>内蒙古</t>
+  </si>
+  <si>
+    <t>英语月份的缩写</t>
+  </si>
+  <si>
+    <t>美式英語是要以 月/日/年</t>
+  </si>
+  <si>
+    <t>英式英語是要以 日/月/年</t>
+  </si>
+  <si>
+    <t>中國語文是以年/月/日</t>
+  </si>
+  <si>
+    <t>January (Jan.) 一月；</t>
+  </si>
+  <si>
+    <t>February (Feb.) 二月；</t>
+  </si>
+  <si>
+    <t>March (Mar.) 三月；</t>
+  </si>
+  <si>
+    <t>April (Apr.) 四月；</t>
+  </si>
+  <si>
+    <t>May (may.)五月；</t>
+  </si>
+  <si>
+    <t>June(Jun.)六月；</t>
+  </si>
+  <si>
+    <t>July(Jul.)七月；</t>
+  </si>
+  <si>
+    <t>August(Aug.)八月；</t>
+  </si>
+  <si>
+    <t>September(Sept.)九月；</t>
+  </si>
+  <si>
+    <t>October(Oct.)十月；</t>
+  </si>
+  <si>
+    <t>November(Nov.)十一月；</t>
+  </si>
+  <si>
+    <t>December(Dec.)十二月 .</t>
+  </si>
+  <si>
+    <t>後面要打點(.)啊</t>
+  </si>
+  <si>
+    <t>[ˈdʒænjuˌɛri]</t>
+  </si>
+  <si>
+    <t>[ˈfɛbruˌɛri, ˈfɛbju-]</t>
+  </si>
+  <si>
+    <t>[mɑ:rtʃ]</t>
+  </si>
+  <si>
+    <t>[ˈeprəl]</t>
+  </si>
+  <si>
+    <t>[me]</t>
+  </si>
+  <si>
+    <t>[dʒu:n]</t>
+  </si>
+  <si>
+    <t>[dʒʊˈlaɪ]</t>
+  </si>
+  <si>
+    <t>[ɔˈɡʌst]</t>
+  </si>
+  <si>
+    <t>[sɛpˈtɛmbɚ]</t>
+  </si>
+  <si>
+    <t>[ɑkˈtobɚ]</t>
+  </si>
+  <si>
+    <t>[noˈvɛmbɚ]</t>
+  </si>
+  <si>
+    <t>[dɪˈsɛmbɚ]</t>
+  </si>
+  <si>
+    <t>還有這些詞不可以用在句子的未尾,且月份的縮寫只有跟日一起用才能縮寫,單獨在句中是不能縮寫</t>
+  </si>
+  <si>
+    <t>常用的星期英文縮寫:</t>
+  </si>
+  <si>
+    <t>星期一： Mon.=Monday</t>
+  </si>
+  <si>
+    <t>星期二： Tues.=Tuesday</t>
+  </si>
+  <si>
+    <t>星期三： Wed.=Wednesday</t>
+  </si>
+  <si>
+    <t>星期五： Fri.=Friday</t>
+  </si>
+  <si>
+    <t>星期六： Sat.=Saturday</t>
+  </si>
+  <si>
+    <t>星期天： Sun.=Sunday</t>
+  </si>
+  <si>
+    <t>[ˈmʌndeɪ]</t>
+  </si>
+  <si>
+    <t>[ˈtuzdi, -ˌde, ˈtjuz-]</t>
+  </si>
+  <si>
+    <t>[ˈwɛnzdi, -ˌde]</t>
+  </si>
+  <si>
+    <t>星期四： Thur.=Thursday</t>
+  </si>
+  <si>
+    <t>[ˈθɚzdi, -ˌde]</t>
+  </si>
+  <si>
+    <t>[ˈfraɪdi, -ˌde]</t>
+  </si>
+  <si>
+    <t>[ˈsætədi, -ˌde]</t>
+  </si>
+  <si>
+    <t>[ˈsʌndi, -ˌde]</t>
+  </si>
+  <si>
+    <t>英語日期中的大寫、縮寫</t>
+  </si>
+  <si>
+    <t>1st 2nd 3rd 4th 5th 6th 7th 8th 9th 10th ；</t>
+  </si>
+  <si>
+    <t>11th 12th 13th 14th 15th 16th 17th 18th 19th 20th ；21st 22nd 23rd 24th 25th 26th 27th 28th 29th 30th 31st</t>
+  </si>
+  <si>
+    <t>注意：正规的英语中六月，七月，九月的缩写是4个字母，其他月份3个字母。挂历上见到的Jun，Jul,Sep是错误的。</t>
+  </si>
+  <si>
+    <t>hundred</t>
+  </si>
+  <si>
+    <t>[ˈhʌndrɪd]</t>
+  </si>
+  <si>
+    <t>thousand</t>
+  </si>
+  <si>
+    <t>[ˈθaʊzənd]</t>
+  </si>
+  <si>
+    <t>billion</t>
+  </si>
+  <si>
+    <t>[ˈbɪljən]</t>
+  </si>
+  <si>
+    <t>million</t>
+  </si>
+  <si>
+    <t>[ˈmɪljən]</t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>[ˈpɚpəl]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adj.紫色的; 帝王的; 词藻华美的; n.紫色; 紫（红）衣，紫袍; 帝位，皇权; 皇族; </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1496,6 +1904,23 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFE7432F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="SimSun"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1518,7 +1943,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1535,6 +1960,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1837,10 +2268,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R188"/>
+  <dimension ref="A1:R216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="B188" sqref="B188"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B219" sqref="B219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3921,6 +4352,286 @@
         <v>473</v>
       </c>
     </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="10" t="s">
+        <v>474</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="D191" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>477</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="D192" s="2" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>480</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="D193" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>483</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="D194" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>486</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="D195" s="2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>489</v>
+      </c>
+      <c r="D196" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A197" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="D197" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A198" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D198" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>494</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D199" s="2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>497</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="D200" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>509</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="D201" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A202" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D202" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>503</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="D203" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>506</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="D204" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>512</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D205" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A206" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="D206" s="2" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>518</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="D207" s="2" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="11" t="s">
+        <v>521</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="D208" s="2" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>524</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="D209" s="2" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>530</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="D210" s="2" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>533</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="D211" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>536</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="D212" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>539</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="D213" s="2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="11" t="s">
+        <v>542</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D214" s="2" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>545</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="D215" s="2" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>548</v>
+      </c>
+      <c r="D216" s="9" t="s">
+        <v>549</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B54" r:id="rId1" display="http://fanyi.baidu.com/"/>
@@ -3936,9 +4647,15 @@
     <hyperlink ref="B160" r:id="rId11" display="http://fanyi.baidu.com/"/>
     <hyperlink ref="B175" r:id="rId12" display="http://fanyi.baidu.com/"/>
     <hyperlink ref="B186" r:id="rId13" display="http://fanyi.baidu.com/"/>
+    <hyperlink ref="B193" r:id="rId14" display="http://fanyi.baidu.com/"/>
+    <hyperlink ref="B194" r:id="rId15" display="http://fanyi.baidu.com/"/>
+    <hyperlink ref="B200" r:id="rId16" display="http://fanyi.baidu.com/"/>
+    <hyperlink ref="B201" r:id="rId17" display="http://fanyi.baidu.com/"/>
+    <hyperlink ref="B209" r:id="rId18" display="http://fanyi.baidu.com/"/>
+    <hyperlink ref="B213" r:id="rId19" display="http://fanyi.baidu.com/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -3947,7 +4664,7 @@
   <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3997,12 +4714,271 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>554</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>555</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>556</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>557</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="D9" s="13"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>558</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>559</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>560</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>561</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>562</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>563</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>564</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>565</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>581</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>582</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="12" t="s">
+        <v>583</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>590</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>584</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>585</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>586</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>599</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>601</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>605</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>603</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>607</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>